<commit_message>
fleshed out start of test object and what gets put where from the test excel file. Just started writing some basic nose tests.
</commit_message>
<xml_diff>
--- a/Tests/1/Test - Single Run.xlsx
+++ b/Tests/1/Test - Single Run.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Vial #</t>
   </si>
@@ -59,9 +59,6 @@
     <t>r2</t>
   </si>
   <si>
-    <t>END OBJ REG</t>
-  </si>
-  <si>
     <t>r2_p1</t>
   </si>
   <si>
@@ -75,6 +72,12 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>END OBJ REG (Index)</t>
+  </si>
+  <si>
+    <t>r2_p2</t>
   </si>
 </sst>
 </file>
@@ -867,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N259"/>
+  <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G274" sqref="G274:G275"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:N69" si="0">C10*C$6</f>
+        <f t="shared" ref="C41:C69" si="0">C10*C$6</f>
         <v>18443.801139943582</v>
       </c>
     </row>
@@ -1874,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72:N100" si="1">C41/C$5/($B41-$B40)</f>
+        <f t="shared" ref="C72:C100" si="1">C41/C$5/($B41-$B40)</f>
         <v>23639.837400594191</v>
       </c>
     </row>
@@ -2152,7 +2155,7 @@
         <v>2</v>
       </c>
       <c r="C103">
-        <f t="shared" ref="C103:N131" si="2">LOG10(C72)</f>
+        <f t="shared" ref="C103:C131" si="2">LOG10(C72)</f>
         <v>4.3736444850574596</v>
       </c>
     </row>
@@ -3003,15 +3006,15 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C163">
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B164" s="4">
         <v>0</v>
@@ -3167,7 +3170,7 @@
         <v>9</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
@@ -3280,7 +3283,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B195" s="4">
         <v>0</v>
@@ -3466,31 +3469,38 @@
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B226" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B227" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B228" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B229" s="4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C229" s="14">
+        <f>SUM(C166,C198)</f>
+        <v>1.9609807731237103</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B230" s="4">
-        <v>3</v>
+      <c r="B230" s="5">
+        <v>4</v>
       </c>
       <c r="C230" s="14">
-        <f t="shared" ref="C230:N230" si="3">SUM(C166,C198)</f>
-        <v>1.9609807731237103</v>
+        <f>SUM(C167,C199)</f>
+        <v>1.9759100661096691</v>
       </c>
       <c r="D230" s="14"/>
       <c r="E230" s="14"/>
@@ -3505,12 +3515,12 @@
       <c r="N230" s="14"/>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B231" s="5">
-        <v>4</v>
+      <c r="B231" s="4">
+        <v>5</v>
       </c>
       <c r="C231" s="14">
-        <f t="shared" ref="C231:N231" si="4">SUM(C167,C199)</f>
-        <v>1.9759100661096691</v>
+        <f>SUM(C168,C200)</f>
+        <v>1.9786152585991283</v>
       </c>
       <c r="D231" s="14"/>
       <c r="E231" s="14"/>
@@ -3526,11 +3536,11 @@
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B232" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C232" s="14">
-        <f t="shared" ref="C232:N232" si="5">SUM(C168,C200)</f>
-        <v>1.9786152585991283</v>
+        <f>SUM(C169,C201)</f>
+        <v>1.9656923464425582</v>
       </c>
       <c r="D232" s="14"/>
       <c r="E232" s="14"/>
@@ -3546,11 +3556,11 @@
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B233" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C233" s="14">
-        <f t="shared" ref="C233:N233" si="6">SUM(C169,C201)</f>
-        <v>1.9656923464425582</v>
+        <f>SUM(C170,C202)</f>
+        <v>1.9553370701163502</v>
       </c>
       <c r="D233" s="14"/>
       <c r="E233" s="14"/>
@@ -3566,11 +3576,11 @@
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B234" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C234" s="14">
-        <f t="shared" ref="C234:N234" si="7">SUM(C170,C202)</f>
-        <v>1.9553370701163502</v>
+        <f>SUM(C171,C203)</f>
+        <v>1.9422998378720693</v>
       </c>
       <c r="D234" s="14"/>
       <c r="E234" s="14"/>
@@ -3586,11 +3596,11 @@
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B235" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C235" s="14">
-        <f t="shared" ref="C235:N235" si="8">SUM(C171,C203)</f>
-        <v>1.9422998378720693</v>
+        <f>SUM(C172,C204)</f>
+        <v>1.93978169515798</v>
       </c>
       <c r="D235" s="14"/>
       <c r="E235" s="14"/>
@@ -3605,12 +3615,8 @@
       <c r="N235" s="14"/>
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B236" s="4">
-        <v>9</v>
-      </c>
-      <c r="C236" s="14">
-        <f t="shared" ref="C236:N236" si="9">SUM(C172,C204)</f>
-        <v>1.93978169515798</v>
+      <c r="B236" s="5">
+        <v>10</v>
       </c>
       <c r="D236" s="14"/>
       <c r="E236" s="14"/>
@@ -3626,107 +3632,111 @@
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B237" s="5">
-        <v>10</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B238" s="5">
-        <v>11.5</v>
+      <c r="B238" s="4">
+        <v>13</v>
       </c>
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B239" s="4">
-        <v>13</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B240" s="4">
-        <v>14.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" s="4">
-        <v>16</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" s="4">
-        <v>17.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" s="4">
-        <v>19</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" s="4">
-        <v>20.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" s="4">
-        <v>22</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" s="4">
-        <v>23.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" s="4">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" s="4">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" s="4">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" s="4">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" s="4">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B257" s="4">
-        <v>45</v>
+      <c r="A257" t="s">
+        <v>16</v>
+      </c>
+      <c r="C257">
+        <f>MAX(C226:C256)</f>
+        <v>1.9786152585991283</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -3734,16 +3744,7 @@
         <v>17</v>
       </c>
       <c r="C258">
-        <f>MAX(C227:C257)</f>
-        <v>1.9786152585991283</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>18</v>
-      </c>
-      <c r="C259">
-        <f>MATCH(C258,C228:C257,0)</f>
+        <f>MATCH(C257,C227:C256,0)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented basic tests. Now time to look at bigger picture sutff: archetecture of experiment/analysis objects and how analyses are handeled. Or just do tests for multiple runs -\_(-_-)_/-
</commit_message>
<xml_diff>
--- a/Tests/1/Test - Single Run.xlsx
+++ b/Tests/1/Test - Single Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C225" sqref="C225"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G205" sqref="G205:G206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
created Phase object for holding individual phase data. Finished phase 3 analysis
</commit_message>
<xml_diff>
--- a/Tests/1/Test - Single Run.xlsx
+++ b/Tests/1/Test - Single Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
@@ -10,7 +10,7 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Answers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" calcOnSave="0"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G205" sqref="G205:G206"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G205" sqref="G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="C229" s="14">
-        <f>SUM(C166,C198)</f>
+        <f t="shared" ref="C229:C235" si="3">SUM(C166,C198)</f>
         <v>1.9609807731237103</v>
       </c>
     </row>
@@ -3499,7 +3499,7 @@
         <v>4</v>
       </c>
       <c r="C230" s="14">
-        <f>SUM(C167,C199)</f>
+        <f t="shared" si="3"/>
         <v>1.9759100661096691</v>
       </c>
       <c r="D230" s="14"/>
@@ -3519,7 +3519,7 @@
         <v>5</v>
       </c>
       <c r="C231" s="14">
-        <f>SUM(C168,C200)</f>
+        <f t="shared" si="3"/>
         <v>1.9786152585991283</v>
       </c>
       <c r="D231" s="14"/>
@@ -3539,7 +3539,7 @@
         <v>6</v>
       </c>
       <c r="C232" s="14">
-        <f>SUM(C169,C201)</f>
+        <f t="shared" si="3"/>
         <v>1.9656923464425582</v>
       </c>
       <c r="D232" s="14"/>
@@ -3559,7 +3559,7 @@
         <v>7</v>
       </c>
       <c r="C233" s="14">
-        <f>SUM(C170,C202)</f>
+        <f t="shared" si="3"/>
         <v>1.9553370701163502</v>
       </c>
       <c r="D233" s="14"/>
@@ -3579,7 +3579,7 @@
         <v>8</v>
       </c>
       <c r="C234" s="14">
-        <f>SUM(C171,C203)</f>
+        <f t="shared" si="3"/>
         <v>1.9422998378720693</v>
       </c>
       <c r="D234" s="14"/>
@@ -3599,7 +3599,7 @@
         <v>9</v>
       </c>
       <c r="C235" s="14">
-        <f>SUM(C172,C204)</f>
+        <f t="shared" si="3"/>
         <v>1.93978169515798</v>
       </c>
       <c r="D235" s="14"/>

</xml_diff>

<commit_message>
finished most mating of data with GUI. Started writing tests! Needed to refactor Operations.py for testing'
</commit_message>
<xml_diff>
--- a/Tests/1/Test - Single Run.xlsx
+++ b/Tests/1/Test - Single Run.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Vial #</t>
   </si>
@@ -68,16 +68,13 @@
     <t>p12_r2_max</t>
   </si>
   <si>
-    <t>p12_r2_max_row</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>END OBJ REG (Index)</t>
   </si>
   <si>
     <t>r2_p2</t>
+  </si>
+  <si>
+    <t>p12_r2_max_index</t>
   </si>
 </sst>
 </file>
@@ -200,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +227,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G205" sqref="G205"/>
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D259" sqref="D259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2624,7 @@
       <c r="B143" s="5">
         <v>11.5</v>
       </c>
-      <c r="C143" s="15">
+      <c r="C143" s="17">
         <f>RSQ($B112:$B$131, $C112:$C$131)</f>
         <v>0.79592317065125329</v>
       </c>
@@ -3006,10 +3007,10 @@
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C163">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
@@ -3169,8 +3170,9 @@
       <c r="B173" s="4">
         <v>9</v>
       </c>
-      <c r="C173" s="14" t="s">
-        <v>18</v>
+      <c r="C173" s="14">
+        <f>RSQ($B$102:$B110, $C$102:$C110)</f>
+        <v>0.92541062921847905</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
@@ -3180,10 +3182,10 @@
       <c r="C174" s="14"/>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B175" s="5">
+      <c r="B175" s="18">
         <v>11.5</v>
       </c>
-      <c r="C175" s="14"/>
+      <c r="C175" s="15"/>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B176" s="4">
@@ -3283,7 +3285,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B195" s="4">
         <v>0</v>
@@ -3368,9 +3370,10 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B206" s="5">
+      <c r="B206" s="18">
         <v>11.5</v>
       </c>
+      <c r="C206" s="19"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" s="4">
@@ -3490,7 +3493,7 @@
         <v>3</v>
       </c>
       <c r="C229" s="14">
-        <f t="shared" ref="C229:C235" si="3">SUM(C166,C198)</f>
+        <f>SUM(C166,C198)</f>
         <v>1.9609807731237103</v>
       </c>
     </row>
@@ -3499,7 +3502,7 @@
         <v>4</v>
       </c>
       <c r="C230" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C229:C235" si="3">SUM(C167,C199)</f>
         <v>1.9759100661096691</v>
       </c>
       <c r="D230" s="14"/>
@@ -3518,8 +3521,8 @@
       <c r="B231" s="4">
         <v>5</v>
       </c>
-      <c r="C231" s="14">
-        <f t="shared" si="3"/>
+      <c r="C231" s="20">
+        <f>SUM(C168,C200)</f>
         <v>1.9786152585991283</v>
       </c>
       <c r="D231" s="14"/>
@@ -3741,11 +3744,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C258">
-        <f>MATCH(C257,C227:C256,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3758,5 +3760,6 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished implementing some higher level tests. Will probably have to create some test cases from hand (not from previous program)
</commit_message>
<xml_diff>
--- a/Tests/1/Test - Single Run.xlsx
+++ b/Tests/1/Test - Single Run.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Vial #</t>
   </si>
@@ -76,6 +76,39 @@
   <si>
     <t>p12_r2_max_index</t>
   </si>
+  <si>
+    <t>Influx</t>
+  </si>
+  <si>
+    <t>Efflux</t>
+  </si>
+  <si>
+    <t>Net Flux</t>
+  </si>
+  <si>
+    <t>E:I Ratio</t>
+  </si>
+  <si>
+    <t>Pool size</t>
+  </si>
+  <si>
+    <t>Half-life</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -85,7 +118,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +144,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -193,11 +237,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,17 +269,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,55 +618,55 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="24"/>
       <c r="C2">
         <v>17875.075000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="10">
-        <v>8346.5</v>
+      <c r="B3" s="24"/>
+      <c r="C3" s="27">
+        <v>8554.2999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="10">
-        <v>1860.6</v>
+      <c r="B4" s="24"/>
+      <c r="C4" s="28">
+        <v>2770</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="12">
         <v>0.78019999999999978</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="6">
         <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="7">
         <v>60</v>
       </c>
@@ -871,10 +937,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N258"/>
+  <dimension ref="A1:N265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D259" sqref="D259"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,10 +956,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="24"/>
       <c r="C2">
         <v>17875.075000000001</v>
       </c>
@@ -910,12 +976,12 @@
       <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="10">
-        <v>8346.5</v>
+      <c r="B3" s="24"/>
+      <c r="C3">
+        <v>8554.2999999999993</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -930,12 +996,12 @@
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="10">
-        <v>1860.6</v>
+      <c r="B4" s="24"/>
+      <c r="C4">
+        <v>2770</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -950,10 +1016,10 @@
       <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="12">
         <v>0.78019999999999978</v>
       </c>
@@ -970,19 +1036,19 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="6">
         <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="7">
         <v>60</v>
       </c>
@@ -998,156 +1064,160 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="21">
+        <v>2.1149241924285889</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="21">
+        <v>1.4440677165985107</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="21">
+        <v>0.67085647583007813</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="21">
+        <v>0.68279880285263062</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="21">
+        <v>21.277021408081055</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="21">
+        <v>20.915608693201449</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="21">
+        <v>0.79592317342758179</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>47976.6</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8">
-        <v>17743.599999999999</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8">
-        <v>5925</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8">
-        <v>2974.6</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1741</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>6</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1226.0999999999999</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>7</v>
-      </c>
-      <c r="C15" s="8">
-        <v>815.2</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C16" s="8">
-        <v>650.5</v>
+        <v>47976.6</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1163,10 +1233,10 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C17" s="8">
-        <v>527.6</v>
+        <v>17743.599999999999</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -1181,11 +1251,11 @@
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
-        <v>10</v>
+      <c r="B18" s="4">
+        <v>3</v>
       </c>
       <c r="C18" s="8">
-        <v>388.2</v>
+        <v>5925</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -1201,10 +1271,10 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <v>11.5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="8">
-        <v>369.6</v>
+        <v>2974.6</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -1220,10 +1290,10 @@
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" s="8">
-        <v>349.5</v>
+        <v>1741</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1239,10 +1309,10 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <v>14.5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="8">
-        <v>301.89999999999998</v>
+        <v>1226.0999999999999</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -1258,10 +1328,10 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C22" s="8">
-        <v>288</v>
+        <v>815.2</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -1277,10 +1347,10 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
-        <v>17.5</v>
+        <v>8</v>
       </c>
       <c r="C23" s="8">
-        <v>235.3</v>
+        <v>650.5</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -1296,10 +1366,10 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C24" s="8">
-        <v>220.7</v>
+        <v>527.6</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1314,11 +1384,11 @@
       <c r="N24" s="10"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>20.5</v>
+      <c r="B25" s="5">
+        <v>10</v>
       </c>
       <c r="C25" s="8">
-        <v>167.9</v>
+        <v>388.2</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -1333,11 +1403,11 @@
       <c r="N25" s="10"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>22</v>
+      <c r="B26" s="5">
+        <v>11.5</v>
       </c>
       <c r="C26" s="8">
-        <v>175.9</v>
+        <v>369.6</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -1353,10 +1423,10 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
-        <v>23.5</v>
+        <v>13</v>
       </c>
       <c r="C27" s="8">
-        <v>165.1</v>
+        <v>349.5</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -1372,10 +1442,10 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
-        <v>25</v>
+        <v>14.5</v>
       </c>
       <c r="C28" s="8">
-        <v>143</v>
+        <v>301.89999999999998</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1385,15 +1455,16 @@
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C29" s="8">
-        <v>180.4</v>
+        <v>288</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1409,10 +1480,10 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
-        <v>29</v>
+        <v>17.5</v>
       </c>
       <c r="C30" s="8">
-        <v>167.1</v>
+        <v>235.3</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -1428,10 +1499,10 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C31" s="8">
-        <v>174.5</v>
+        <v>220.7</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -1447,10 +1518,10 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
-        <v>33</v>
+        <v>20.5</v>
       </c>
       <c r="C32" s="8">
-        <v>188.2</v>
+        <v>167.9</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1466,10 +1537,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C33" s="8">
-        <v>160.4</v>
+        <v>175.9</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -1485,10 +1556,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
-        <v>37</v>
+        <v>23.5</v>
       </c>
       <c r="C34" s="8">
-        <v>164.5</v>
+        <v>165.1</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -1504,10 +1575,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C35" s="8">
-        <v>175.2</v>
+        <v>143</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -1517,16 +1588,15 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C36" s="8">
-        <v>177.7</v>
+        <v>180.4</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -1542,10 +1612,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C37" s="8">
-        <v>165</v>
+        <v>167.1</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -1561,10 +1631,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C38" s="8">
-        <v>137.1</v>
+        <v>174.5</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -1579,994 +1649,987 @@
       <c r="N38" s="10"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>11</v>
-      </c>
       <c r="B39" s="4">
-        <v>0</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C39" s="8">
+        <v>188.2</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <f>C9*C$6</f>
-        <v>49869.861232817311</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C40" s="8">
+        <v>160.4</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <f t="shared" ref="C41:C69" si="0">C10*C$6</f>
-        <v>18443.801139943582</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C41" s="8">
+        <v>164.5</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
+        <v>39</v>
+      </c>
+      <c r="C42" s="8">
+        <v>175.2</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>41</v>
+      </c>
+      <c r="C43" s="8">
+        <v>177.7</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>43</v>
+      </c>
+      <c r="C44" s="8">
+        <v>165</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>45</v>
+      </c>
+      <c r="C45" s="8">
+        <v>137.1</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <f>C16*C$6</f>
+        <v>49869.861232817311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:C76" si="0">C17*C$6</f>
+        <v>18443.801139943582</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
         <v>3</v>
       </c>
-      <c r="C42">
+      <c r="C49">
         <f t="shared" si="0"/>
         <v>6158.8134174669021</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="5">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
         <v>4</v>
       </c>
-      <c r="C43">
+      <c r="C50">
         <f t="shared" si="0"/>
         <v>3091.9842011134256</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="4">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
         <v>5</v>
       </c>
-      <c r="C44">
+      <c r="C51">
         <f t="shared" si="0"/>
         <v>1809.7036556641142</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
         <v>6</v>
       </c>
-      <c r="C45">
+      <c r="C52">
         <f t="shared" si="0"/>
         <v>1274.4845790980876</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
         <v>7</v>
       </c>
-      <c r="C46">
+      <c r="C53">
         <f t="shared" si="0"/>
         <v>847.3695692690327</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="4">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
         <v>8</v>
       </c>
-      <c r="C47">
+      <c r="C54">
         <f t="shared" si="0"/>
         <v>676.17014819615531</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="4">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
         <v>9</v>
       </c>
-      <c r="C48">
+      <c r="C55">
         <f t="shared" si="0"/>
         <v>548.4202462540992</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="5">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
         <v>10</v>
       </c>
-      <c r="C49">
+      <c r="C56">
         <f t="shared" si="0"/>
         <v>403.51921833935046</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="5">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
         <v>11.5</v>
       </c>
-      <c r="C50">
+      <c r="C57">
         <f t="shared" si="0"/>
         <v>384.18522178831512</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
         <v>13</v>
       </c>
-      <c r="C51">
+      <c r="C58">
         <f t="shared" si="0"/>
         <v>363.29203196703497</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
         <v>14.5</v>
       </c>
-      <c r="C52">
+      <c r="C59">
         <f t="shared" si="0"/>
         <v>313.81363219126712</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="4">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
         <v>16</v>
       </c>
-      <c r="C53">
+      <c r="C60">
         <f t="shared" si="0"/>
         <v>299.36510788699877</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="4">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="4">
         <v>17.5</v>
       </c>
-      <c r="C54">
+      <c r="C61">
         <f t="shared" si="0"/>
         <v>244.58545099239868</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="4">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="4">
         <v>19</v>
       </c>
-      <c r="C55">
+      <c r="C62">
         <f t="shared" si="0"/>
         <v>229.40930316201607</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="4">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="4">
         <v>20.5</v>
       </c>
-      <c r="C56">
+      <c r="C63">
         <f t="shared" si="0"/>
         <v>174.52570004939966</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="4">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="4">
         <v>22</v>
       </c>
-      <c r="C57">
+      <c r="C64">
         <f t="shared" si="0"/>
         <v>182.84139749070516</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
         <v>23.5</v>
       </c>
-      <c r="C58">
+      <c r="C65">
         <f t="shared" si="0"/>
         <v>171.61520594494272</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
         <v>25</v>
       </c>
-      <c r="C59">
+      <c r="C66">
         <f t="shared" si="0"/>
         <v>148.6430917633362</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="4">
         <v>27</v>
       </c>
-      <c r="C60">
+      <c r="C67">
         <f t="shared" si="0"/>
         <v>187.51897730143952</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="4">
         <v>29</v>
       </c>
-      <c r="C61">
+      <c r="C68">
         <f t="shared" si="0"/>
         <v>173.69413030526908</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="4">
         <v>31</v>
       </c>
-      <c r="C62">
+      <c r="C69">
         <f t="shared" si="0"/>
         <v>181.3861504384767</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="4">
         <v>33</v>
       </c>
-      <c r="C63">
+      <c r="C70">
         <f t="shared" si="0"/>
         <v>195.62678230671239</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="4">
         <v>35</v>
       </c>
-      <c r="C64">
+      <c r="C71">
         <f t="shared" si="0"/>
         <v>166.72973369817572</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="4">
         <v>37</v>
       </c>
-      <c r="C65">
+      <c r="C72">
         <f t="shared" si="0"/>
         <v>170.99152863684481</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="4">
         <v>39</v>
       </c>
-      <c r="C66">
+      <c r="C73">
         <f t="shared" si="0"/>
         <v>182.11377396459093</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="4">
         <v>41</v>
       </c>
-      <c r="C67">
+      <c r="C74">
         <f t="shared" si="0"/>
         <v>184.71242941499889</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="4">
         <v>43</v>
       </c>
-      <c r="C68">
+      <c r="C75">
         <f t="shared" si="0"/>
         <v>171.5112597269264</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="4">
         <v>45</v>
       </c>
-      <c r="C69">
+      <c r="C76">
         <f t="shared" si="0"/>
         <v>142.51026490037339</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B77" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="4">
         <v>1</v>
       </c>
-      <c r="C71">
-        <f>C40/C$5/($B40-$B39)</f>
+      <c r="C78">
+        <f>C47/C$5/($B47-$B46)</f>
         <v>63919.329957469017</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="4">
         <v>2</v>
       </c>
-      <c r="C72">
-        <f t="shared" ref="C72:C100" si="1">C41/C$5/($B41-$B40)</f>
+      <c r="C79">
+        <f t="shared" ref="C79:C107" si="1">C48/C$5/($B48-$B47)</f>
         <v>23639.837400594191</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
         <v>3</v>
       </c>
-      <c r="C73">
+      <c r="C80">
         <f t="shared" si="1"/>
         <v>7893.8905632746782</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="5">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="5">
         <v>4</v>
       </c>
-      <c r="C74">
+      <c r="C81">
         <f t="shared" si="1"/>
         <v>3963.0661383150814</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="4">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
         <v>5</v>
       </c>
-      <c r="C75">
+      <c r="C82">
         <f t="shared" si="1"/>
         <v>2319.5381385082219</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="4">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="4">
         <v>6</v>
       </c>
-      <c r="C76">
+      <c r="C83">
         <f t="shared" si="1"/>
         <v>1633.5357332710689</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="4">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="4">
         <v>7</v>
       </c>
-      <c r="C77">
+      <c r="C84">
         <f t="shared" si="1"/>
         <v>1086.092757330214</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="4">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="4">
         <v>8</v>
       </c>
-      <c r="C78">
+      <c r="C85">
         <f t="shared" si="1"/>
         <v>866.66258420424958</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="4">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="4">
         <v>9</v>
       </c>
-      <c r="C79">
+      <c r="C86">
         <f t="shared" si="1"/>
         <v>702.92264323775873</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="5">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="5">
         <v>10</v>
       </c>
-      <c r="C80">
+      <c r="C87">
         <f t="shared" si="1"/>
         <v>517.19971589252827</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="5">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="5">
         <v>11.5</v>
       </c>
-      <c r="C81">
+      <c r="C88">
         <f t="shared" si="1"/>
         <v>328.27926325584485</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="4">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="4">
         <v>13</v>
       </c>
-      <c r="C82">
+      <c r="C89">
         <f t="shared" si="1"/>
         <v>310.4264137118987</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="4">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="4">
         <v>14.5</v>
       </c>
-      <c r="C83">
+      <c r="C90">
         <f t="shared" si="1"/>
         <v>268.14802374713082</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="4">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="4">
         <v>16</v>
       </c>
-      <c r="C84">
+      <c r="C91">
         <f t="shared" si="1"/>
         <v>255.80202331624272</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="4">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="4">
         <v>17.5</v>
       </c>
-      <c r="C85">
+      <c r="C92">
         <f t="shared" si="1"/>
         <v>208.99380585524969</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="4">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="4">
         <v>19</v>
       </c>
-      <c r="C86">
+      <c r="C93">
         <f t="shared" si="1"/>
         <v>196.02606439546796</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="4">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="4">
         <v>20.5</v>
       </c>
-      <c r="C87">
+      <c r="C94">
         <f t="shared" si="1"/>
         <v>149.12902678749015</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="4">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="4">
         <v>22</v>
       </c>
-      <c r="C88">
+      <c r="C95">
         <f t="shared" si="1"/>
         <v>156.23463854627462</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="4">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="4">
         <v>23.5</v>
       </c>
-      <c r="C89">
+      <c r="C96">
         <f t="shared" si="1"/>
         <v>146.64206267191554</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="4">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="4">
         <v>25</v>
       </c>
-      <c r="C90">
+      <c r="C97">
         <f t="shared" si="1"/>
         <v>127.01281018827331</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="4">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="4">
         <v>27</v>
       </c>
-      <c r="C91">
+      <c r="C98">
         <f t="shared" si="1"/>
         <v>120.17365887044321</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="4">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="4">
         <v>29</v>
       </c>
-      <c r="C92">
+      <c r="C99">
         <f t="shared" si="1"/>
         <v>111.31384920870875</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="4">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="4">
         <v>31</v>
       </c>
-      <c r="C93">
+      <c r="C100">
         <f t="shared" si="1"/>
         <v>116.24336736636552</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="4">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="4">
         <v>33</v>
       </c>
-      <c r="C94">
+      <c r="C101">
         <f t="shared" si="1"/>
         <v>125.36963746905437</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="4">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="4">
         <v>35</v>
       </c>
-      <c r="C95">
+      <c r="C102">
         <f t="shared" si="1"/>
         <v>106.85063682272224</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="4">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="4">
         <v>37</v>
       </c>
-      <c r="C96">
+      <c r="C103">
         <f t="shared" si="1"/>
         <v>109.58185634250503</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="4">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4">
         <v>39</v>
       </c>
-      <c r="C97">
+      <c r="C104">
         <f t="shared" si="1"/>
         <v>116.70967313803575</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="4">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="4">
         <v>41</v>
       </c>
-      <c r="C98">
+      <c r="C105">
         <f t="shared" si="1"/>
         <v>118.37505089400086</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="4">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="4">
         <v>43</v>
       </c>
-      <c r="C99">
+      <c r="C106">
         <f t="shared" si="1"/>
         <v>109.91493189369805</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="4">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="4">
         <v>45</v>
       </c>
-      <c r="C100">
+      <c r="C107">
         <f t="shared" si="1"/>
         <v>91.329316137127293</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>12</v>
       </c>
-      <c r="B101" s="4">
+      <c r="B108" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="4">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="4">
         <v>1</v>
       </c>
-      <c r="C102">
-        <f>LOG10(C71)</f>
+      <c r="C109">
+        <f>LOG10(C78)</f>
         <v>4.8056322137824834</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="4">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="4">
         <v>2</v>
       </c>
-      <c r="C103">
-        <f t="shared" ref="C103:C131" si="2">LOG10(C72)</f>
+      <c r="C110">
+        <f t="shared" ref="C110:C138" si="2">LOG10(C79)</f>
         <v>4.3736444850574596</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="4">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="4">
         <v>3</v>
       </c>
-      <c r="C104">
+      <c r="C111">
         <f t="shared" si="2"/>
         <v>3.8972911012721423</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="5">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="5">
         <v>4</v>
       </c>
-      <c r="C105">
+      <c r="C112">
         <f t="shared" si="2"/>
         <v>3.5980313201932868</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="4">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="4">
         <v>5</v>
       </c>
-      <c r="C106">
+      <c r="C113">
         <f t="shared" si="2"/>
         <v>3.365401517707332</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="4">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="4">
         <v>6</v>
       </c>
-      <c r="C107">
+      <c r="C114">
         <f t="shared" si="2"/>
         <v>3.213128639021257</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="4">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" s="4">
         <v>7</v>
       </c>
-      <c r="C108">
+      <c r="C115">
         <f t="shared" si="2"/>
         <v>3.035866917588371</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="4">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="4">
         <v>8</v>
       </c>
-      <c r="C109">
+      <c r="C116">
         <f t="shared" si="2"/>
         <v>2.9378500474876059</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="4">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="4">
         <v>9</v>
       </c>
-      <c r="C110">
+      <c r="C117">
         <f t="shared" si="2"/>
         <v>2.8469075334643286</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="5">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="5">
         <v>10</v>
       </c>
-      <c r="C111">
+      <c r="C118">
         <f t="shared" si="2"/>
         <v>2.7136582776423448</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="5">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="17">
         <v>11.5</v>
       </c>
-      <c r="C112">
+      <c r="C119" s="18">
         <f t="shared" si="2"/>
         <v>2.5162434500823889</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="4">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="4">
         <v>13</v>
       </c>
-      <c r="C113">
+      <c r="C120">
         <f t="shared" si="2"/>
         <v>2.4919586676160197</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="4">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="4">
         <v>14.5</v>
       </c>
-      <c r="C114">
+      <c r="C121">
         <f t="shared" si="2"/>
         <v>2.4283746005574174</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115" s="4">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="4">
         <v>16</v>
       </c>
-      <c r="C115">
+      <c r="C122">
         <f t="shared" si="2"/>
         <v>2.4079039752935505</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="4">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="4">
         <v>17.5</v>
       </c>
-      <c r="C116">
+      <c r="C123">
         <f t="shared" si="2"/>
         <v>2.320133414710341</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="4">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="4">
         <v>19</v>
       </c>
-      <c r="C117">
+      <c r="C124">
         <f t="shared" si="2"/>
         <v>2.2923138206959748</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="4">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="4">
         <v>20.5</v>
       </c>
-      <c r="C118">
+      <c r="C125">
         <f t="shared" si="2"/>
         <v>2.1735621836723684</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="4">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="4">
         <v>22</v>
       </c>
-      <c r="C119">
+      <c r="C126">
         <f t="shared" si="2"/>
         <v>2.1937773269917811</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="4">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="4">
         <v>23.5</v>
       </c>
-      <c r="C120">
+      <c r="C127">
         <f t="shared" si="2"/>
         <v>2.1662585607971132</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="4">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="4">
         <v>25</v>
       </c>
-      <c r="C121">
+      <c r="C128">
         <f t="shared" si="2"/>
         <v>2.1038475249993813</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="4">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B129" s="4">
         <v>27</v>
       </c>
-      <c r="C122">
+      <c r="C129">
         <f t="shared" si="2"/>
         <v>2.0798092841319429</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="4">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B130" s="4">
         <v>29</v>
       </c>
-      <c r="C123">
+      <c r="C130">
         <f t="shared" si="2"/>
         <v>2.0465492008194111</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="4">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B131" s="4">
         <v>31</v>
       </c>
-      <c r="C124">
+      <c r="C131">
         <f t="shared" si="2"/>
         <v>2.0653681822212184</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="4">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B132" s="4">
         <v>33</v>
       </c>
-      <c r="C125">
+      <c r="C132">
         <f t="shared" si="2"/>
         <v>2.0981923700172578</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B126" s="4">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B133" s="4">
         <v>35</v>
       </c>
-      <c r="C126">
+      <c r="C133">
         <f t="shared" si="2"/>
         <v>2.0287771148741647</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B127" s="4">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B134" s="4">
         <v>37</v>
       </c>
-      <c r="C127">
+      <c r="C134">
         <f t="shared" si="2"/>
         <v>2.0397386532120128</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="4">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B135" s="4">
         <v>39</v>
       </c>
-      <c r="C128">
+      <c r="C135">
         <f t="shared" si="2"/>
         <v>2.0671068527580818</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B129" s="4">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B136" s="4">
         <v>41</v>
       </c>
-      <c r="C129">
+      <c r="C136">
         <f t="shared" si="2"/>
         <v>2.0732601787313212</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B130" s="4">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B137" s="4">
         <v>43</v>
       </c>
-      <c r="C130">
+      <c r="C137">
         <f t="shared" si="2"/>
         <v>2.0410566951399263</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B131" s="4">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B138" s="4">
         <v>45</v>
       </c>
-      <c r="C131">
+      <c r="C138">
         <f t="shared" si="2"/>
         <v>1.9606102057155324</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>13</v>
       </c>
-      <c r="B132" s="4">
+      <c r="B139" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B133" s="4">
-        <v>1</v>
-      </c>
-      <c r="C133" s="14">
-        <f>RSQ($B102:$B$131, $C102:$C$131)</f>
-        <v>0.65069533432746318</v>
-      </c>
-      <c r="D133" s="14"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
-      <c r="G133" s="14"/>
-      <c r="H133" s="14"/>
-      <c r="I133" s="14"/>
-      <c r="J133" s="14"/>
-      <c r="K133" s="14"/>
-      <c r="L133" s="14"/>
-      <c r="M133" s="14"/>
-      <c r="N133" s="14"/>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B134" s="4">
-        <v>2</v>
-      </c>
-      <c r="C134" s="14">
-        <f>RSQ($B103:$B$131, $C103:$C$131)</f>
-        <v>0.67701998606018554</v>
-      </c>
-      <c r="D134" s="14"/>
-      <c r="E134" s="14"/>
-      <c r="F134" s="14"/>
-      <c r="G134" s="14"/>
-      <c r="H134" s="14"/>
-      <c r="I134" s="14"/>
-      <c r="J134" s="14"/>
-      <c r="K134" s="14"/>
-      <c r="L134" s="14"/>
-      <c r="M134" s="14"/>
-      <c r="N134" s="14"/>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B135" s="4">
-        <v>3</v>
-      </c>
-      <c r="C135" s="14">
-        <f>RSQ($B104:$B$131, $C104:$C$131)</f>
-        <v>0.70947004931443236</v>
-      </c>
-      <c r="D135" s="14"/>
-      <c r="E135" s="14"/>
-      <c r="F135" s="14"/>
-      <c r="G135" s="14"/>
-      <c r="H135" s="14"/>
-      <c r="I135" s="14"/>
-      <c r="J135" s="14"/>
-      <c r="K135" s="14"/>
-      <c r="L135" s="14"/>
-      <c r="M135" s="14"/>
-      <c r="N135" s="14"/>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B136" s="5">
-        <v>4</v>
-      </c>
-      <c r="C136" s="14">
-        <f>RSQ($B105:$B$131, $C105:$C$131)</f>
-        <v>0.72781260547155502</v>
-      </c>
-      <c r="D136" s="14"/>
-      <c r="E136" s="14"/>
-      <c r="F136" s="14"/>
-      <c r="G136" s="14"/>
-      <c r="H136" s="14"/>
-      <c r="I136" s="14"/>
-      <c r="J136" s="14"/>
-      <c r="K136" s="14"/>
-      <c r="L136" s="14"/>
-      <c r="M136" s="14"/>
-      <c r="N136" s="14"/>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B137" s="4">
-        <v>5</v>
-      </c>
-      <c r="C137" s="14">
-        <f>RSQ($B106:$B$131, $C106:$C$131)</f>
-        <v>0.73990399899602211</v>
-      </c>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
-      <c r="H137" s="14"/>
-      <c r="I137" s="14"/>
-      <c r="J137" s="14"/>
-      <c r="K137" s="14"/>
-      <c r="L137" s="14"/>
-      <c r="M137" s="14"/>
-      <c r="N137" s="14"/>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B138" s="4">
-        <v>6</v>
-      </c>
-      <c r="C138" s="14">
-        <f>RSQ($B107:$B$131, $C107:$C$131)</f>
-        <v>0.74612673652712536</v>
-      </c>
-      <c r="D138" s="14"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="14"/>
-      <c r="I138" s="14"/>
-      <c r="J138" s="14"/>
-      <c r="K138" s="14"/>
-      <c r="L138" s="14"/>
-      <c r="M138" s="14"/>
-      <c r="N138" s="14"/>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B139" s="4">
-        <v>7</v>
-      </c>
-      <c r="C139" s="14">
-        <f>RSQ($B108:$B$131, $C108:$C$131)</f>
-        <v>0.75422096364882085</v>
-      </c>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
-      <c r="H139" s="14"/>
-      <c r="I139" s="14"/>
-      <c r="J139" s="14"/>
-      <c r="K139" s="14"/>
-      <c r="L139" s="14"/>
-      <c r="M139" s="14"/>
-      <c r="N139" s="14"/>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B140" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C140" s="14">
-        <f>RSQ($B109:$B$131, $C109:$C$131)</f>
-        <v>0.75470568617197564</v>
+        <f>RSQ($B109:$B$138, $C109:$C$138)</f>
+        <v>0.65069533432746318</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
@@ -2582,11 +2645,11 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B141" s="4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C141" s="14">
-        <f>RSQ($B110:$B$131, $C110:$C$131)</f>
-        <v>0.76021971270134547</v>
+        <f>RSQ($B110:$B$138, $C110:$C$138)</f>
+        <v>0.67701998606018554</v>
       </c>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
@@ -2601,12 +2664,12 @@
       <c r="N141" s="14"/>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B142" s="5">
-        <v>10</v>
+      <c r="B142" s="4">
+        <v>3</v>
       </c>
       <c r="C142" s="14">
-        <f>RSQ($B111:$B$131, $C111:$C$131)</f>
-        <v>0.77875926667313866</v>
+        <f>RSQ($B111:$B$138, $C111:$C$138)</f>
+        <v>0.70947004931443236</v>
       </c>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
@@ -2622,31 +2685,31 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B143" s="5">
-        <v>11.5</v>
-      </c>
-      <c r="C143" s="17">
-        <f>RSQ($B112:$B$131, $C112:$C$131)</f>
-        <v>0.79592317065125329</v>
-      </c>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
-      <c r="G143" s="15"/>
-      <c r="H143" s="15"/>
-      <c r="I143" s="15"/>
-      <c r="J143" s="15"/>
-      <c r="K143" s="15"/>
-      <c r="L143" s="15"/>
-      <c r="M143" s="15"/>
-      <c r="N143" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="C143" s="14">
+        <f>RSQ($B112:$B$138, $C112:$C$138)</f>
+        <v>0.72781260547155502</v>
+      </c>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+      <c r="G143" s="14"/>
+      <c r="H143" s="14"/>
+      <c r="I143" s="14"/>
+      <c r="J143" s="14"/>
+      <c r="K143" s="14"/>
+      <c r="L143" s="14"/>
+      <c r="M143" s="14"/>
+      <c r="N143" s="14"/>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B144" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C144" s="14">
-        <f>RSQ($B113:$B$131, $C113:$C$131)</f>
-        <v>0.77386243722722403</v>
+        <f>RSQ($B113:$B$138, $C113:$C$138)</f>
+        <v>0.73990399899602211</v>
       </c>
       <c r="D144" s="14"/>
       <c r="E144" s="14"/>
@@ -2662,11 +2725,11 @@
     </row>
     <row r="145" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B145" s="4">
-        <v>14.5</v>
+        <v>6</v>
       </c>
       <c r="C145" s="14">
-        <f>RSQ($B114:$B$131, $C114:$C$131)</f>
-        <v>0.75582813539225968</v>
+        <f>RSQ($B114:$B$138, $C114:$C$138)</f>
+        <v>0.74612673652712536</v>
       </c>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
@@ -2682,11 +2745,11 @@
     </row>
     <row r="146" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B146" s="4">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C146" s="14">
-        <f>RSQ($B115:$B$131, $C115:$C$131)</f>
-        <v>0.73057295458973015</v>
+        <f>RSQ($B115:$B$138, $C115:$C$138)</f>
+        <v>0.75422096364882085</v>
       </c>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
@@ -2702,11 +2765,11 @@
     </row>
     <row r="147" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B147" s="4">
-        <v>17.5</v>
+        <v>8</v>
       </c>
       <c r="C147" s="14">
-        <f>RSQ($B116:$B$131, $C116:$C$131)</f>
-        <v>0.7249427804717985</v>
+        <f>RSQ($B116:$B$138, $C116:$C$138)</f>
+        <v>0.75470568617197564</v>
       </c>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
@@ -2722,11 +2785,11 @@
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B148" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C148" s="14">
-        <f>RSQ($B117:$B$131, $C117:$C$131)</f>
-        <v>0.69559742167988348</v>
+        <f>RSQ($B117:$B$138, $C117:$C$138)</f>
+        <v>0.76021971270134547</v>
       </c>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
@@ -2741,12 +2804,12 @@
       <c r="N148" s="14"/>
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B149" s="4">
-        <v>20.5</v>
+      <c r="B149" s="5">
+        <v>10</v>
       </c>
       <c r="C149" s="14">
-        <f>RSQ($B118:$B$131, $C118:$C$131)</f>
-        <v>0.68826305070671678</v>
+        <f>RSQ($B118:$B$138, $C118:$C$138)</f>
+        <v>0.77875926667313866</v>
       </c>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
@@ -2761,32 +2824,32 @@
       <c r="N149" s="14"/>
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B150" s="4">
-        <v>22</v>
-      </c>
-      <c r="C150" s="14">
-        <f>RSQ($B119:$B$131, $C119:$C$131)</f>
-        <v>0.62898454927957781</v>
-      </c>
-      <c r="D150" s="14"/>
-      <c r="E150" s="14"/>
-      <c r="F150" s="14"/>
-      <c r="G150" s="14"/>
-      <c r="H150" s="14"/>
-      <c r="I150" s="14"/>
-      <c r="J150" s="14"/>
-      <c r="K150" s="14"/>
-      <c r="L150" s="14"/>
-      <c r="M150" s="14"/>
-      <c r="N150" s="14"/>
+      <c r="B150" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="C150" s="16">
+        <f>RSQ($B119:$B$138, $C119:$C$138)</f>
+        <v>0.79592317065125329</v>
+      </c>
+      <c r="D150" s="15"/>
+      <c r="E150" s="15"/>
+      <c r="F150" s="15"/>
+      <c r="G150" s="15"/>
+      <c r="H150" s="15"/>
+      <c r="I150" s="15"/>
+      <c r="J150" s="15"/>
+      <c r="K150" s="15"/>
+      <c r="L150" s="15"/>
+      <c r="M150" s="15"/>
+      <c r="N150" s="15"/>
     </row>
     <row r="151" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B151" s="4">
-        <v>23.5</v>
+        <v>13</v>
       </c>
       <c r="C151" s="14">
-        <f>RSQ($B120:$B$131, $C120:$C$131)</f>
-        <v>0.54371626190997113</v>
+        <f>RSQ($B120:$B$138, $C120:$C$138)</f>
+        <v>0.77386243722722403</v>
       </c>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
@@ -2802,11 +2865,11 @@
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B152" s="4">
-        <v>25</v>
+        <v>14.5</v>
       </c>
       <c r="C152" s="14">
-        <f>RSQ($B121:$B$131, $C121:$C$131)</f>
-        <v>0.41845307930733983</v>
+        <f>RSQ($B121:$B$138, $C121:$C$138)</f>
+        <v>0.75582813539225968</v>
       </c>
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
@@ -2822,11 +2885,11 @@
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B153" s="4">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C153" s="14">
-        <f>RSQ($B122:$B$131, $C122:$C$131)</f>
-        <v>0.31240814556227225</v>
+        <f>RSQ($B122:$B$138, $C122:$C$138)</f>
+        <v>0.73057295458973015</v>
       </c>
       <c r="D153" s="14"/>
       <c r="E153" s="14"/>
@@ -2842,11 +2905,11 @@
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B154" s="4">
-        <v>29</v>
+        <v>17.5</v>
       </c>
       <c r="C154" s="14">
-        <f>RSQ($B123:$B$131, $C123:$C$131)</f>
-        <v>0.25608028217206363</v>
+        <f>RSQ($B123:$B$138, $C123:$C$138)</f>
+        <v>0.7249427804717985</v>
       </c>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
@@ -2862,11 +2925,11 @@
     </row>
     <row r="155" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B155" s="4">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C155" s="14">
-        <f>RSQ($B124:$B$131, $C124:$C$131)</f>
-        <v>0.36729821972567317</v>
+        <f>RSQ($B124:$B$138, $C124:$C$138)</f>
+        <v>0.69559742167988348</v>
       </c>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
@@ -2882,11 +2945,11 @@
     </row>
     <row r="156" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B156" s="4">
-        <v>33</v>
+        <v>20.5</v>
       </c>
       <c r="C156" s="14">
-        <f>RSQ($B125:$B$131, $C125:$C$131)</f>
-        <v>0.38931719522473118</v>
+        <f>RSQ($B125:$B$138, $C125:$C$138)</f>
+        <v>0.68826305070671678</v>
       </c>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
@@ -2902,11 +2965,11 @@
     </row>
     <row r="157" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B157" s="4">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C157" s="14">
-        <f>RSQ($B126:$B$131, $C126:$C$131)</f>
-        <v>0.19228537287454706</v>
+        <f>RSQ($B126:$B$138, $C126:$C$138)</f>
+        <v>0.62898454927957781</v>
       </c>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
@@ -2922,11 +2985,11 @@
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B158" s="4">
-        <v>37</v>
+        <v>23.5</v>
       </c>
       <c r="C158" s="14">
-        <f>RSQ($B127:$B$131, $C127:$C$131)</f>
-        <v>0.42048771249168099</v>
+        <f>RSQ($B127:$B$138, $C127:$C$138)</f>
+        <v>0.54371626190997113</v>
       </c>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
@@ -2942,11 +3005,11 @@
     </row>
     <row r="159" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B159" s="4">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C159" s="14">
-        <f>RSQ($B128:$B$131, $C128:$C$131)</f>
-        <v>0.76689900758341678</v>
+        <f>RSQ($B128:$B$138, $C128:$C$138)</f>
+        <v>0.41845307930733983</v>
       </c>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
@@ -2962,11 +3025,11 @@
     </row>
     <row r="160" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B160" s="4">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C160" s="14">
-        <f>RSQ($B129:$B$131, $C129:$C$131)</f>
-        <v>0.94238774061063946</v>
+        <f>RSQ($B129:$B$138, $C129:$C$138)</f>
+        <v>0.31240814556227225</v>
       </c>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
@@ -2982,11 +3045,11 @@
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B161" s="4">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C161" s="14">
-        <f>RSQ($B130:$B$131, $C130:$C$131)</f>
-        <v>1</v>
+        <f>RSQ($B130:$B$138, $C130:$C$138)</f>
+        <v>0.25608028217206363</v>
       </c>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
@@ -3002,37 +3065,91 @@
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B162" s="4">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C162" s="14">
+        <f>RSQ($B131:$B$138, $C131:$C$138)</f>
+        <v>0.36729821972567317</v>
+      </c>
+      <c r="D162" s="14"/>
+      <c r="E162" s="14"/>
+      <c r="F162" s="14"/>
+      <c r="G162" s="14"/>
+      <c r="H162" s="14"/>
+      <c r="I162" s="14"/>
+      <c r="J162" s="14"/>
+      <c r="K162" s="14"/>
+      <c r="L162" s="14"/>
+      <c r="M162" s="14"/>
+      <c r="N162" s="14"/>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>17</v>
-      </c>
-      <c r="C163">
-        <v>11</v>
-      </c>
+      <c r="B163" s="4">
+        <v>33</v>
+      </c>
+      <c r="C163" s="14">
+        <f>RSQ($B132:$B$138, $C132:$C$138)</f>
+        <v>0.38931719522473118</v>
+      </c>
+      <c r="D163" s="14"/>
+      <c r="E163" s="14"/>
+      <c r="F163" s="14"/>
+      <c r="G163" s="14"/>
+      <c r="H163" s="14"/>
+      <c r="I163" s="14"/>
+      <c r="J163" s="14"/>
+      <c r="K163" s="14"/>
+      <c r="L163" s="14"/>
+      <c r="M163" s="14"/>
+      <c r="N163" s="14"/>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>14</v>
-      </c>
       <c r="B164" s="4">
-        <v>0</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C164" s="14">
+        <f>RSQ($B133:$B$138, $C133:$C$138)</f>
+        <v>0.19228537287454706</v>
+      </c>
+      <c r="D164" s="14"/>
+      <c r="E164" s="14"/>
+      <c r="F164" s="14"/>
+      <c r="G164" s="14"/>
+      <c r="H164" s="14"/>
+      <c r="I164" s="14"/>
+      <c r="J164" s="14"/>
+      <c r="K164" s="14"/>
+      <c r="L164" s="14"/>
+      <c r="M164" s="14"/>
+      <c r="N164" s="14"/>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B165" s="4">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C165" s="14">
+        <f>RSQ($B134:$B$138, $C134:$C$138)</f>
+        <v>0.42048771249168099</v>
+      </c>
+      <c r="D165" s="14"/>
+      <c r="E165" s="14"/>
+      <c r="F165" s="14"/>
+      <c r="G165" s="14"/>
+      <c r="H165" s="14"/>
+      <c r="I165" s="14"/>
+      <c r="J165" s="14"/>
+      <c r="K165" s="14"/>
+      <c r="L165" s="14"/>
+      <c r="M165" s="14"/>
+      <c r="N165" s="14"/>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B166" s="4">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="C166" s="14">
-        <f>RSQ($B$102:$B103, $C$102:$C103)</f>
-        <v>0.99999999999999978</v>
+        <f>RSQ($B135:$B$138, $C135:$C$138)</f>
+        <v>0.76689900758341678</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
@@ -3048,11 +3165,11 @@
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B167" s="4">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="C167" s="14">
-        <f>RSQ($B$102:$B104, $C$102:$C104)</f>
-        <v>0.99920543508020454</v>
+        <f>RSQ($B136:$B$138, $C136:$C$138)</f>
+        <v>0.94238774061063946</v>
       </c>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
@@ -3067,12 +3184,12 @@
       <c r="N167" s="14"/>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B168" s="5">
-        <v>4</v>
+      <c r="B168" s="4">
+        <v>43</v>
       </c>
       <c r="C168" s="14">
-        <f>RSQ($B$102:$B105, $C$102:$C105)</f>
-        <v>0.99190519137745259</v>
+        <f>RSQ($B137:$B$138, $C137:$C$138)</f>
+        <v>1</v>
       </c>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
@@ -3088,676 +3205,766 @@
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B169" s="4">
-        <v>5</v>
-      </c>
-      <c r="C169" s="14">
-        <f>RSQ($B$102:$B106, $C$102:$C106)</f>
-        <v>0.98056854197001708</v>
-      </c>
-      <c r="D169" s="14"/>
-      <c r="E169" s="14"/>
-      <c r="F169" s="14"/>
-      <c r="G169" s="14"/>
-      <c r="H169" s="14"/>
-      <c r="I169" s="14"/>
-      <c r="J169" s="14"/>
-      <c r="K169" s="14"/>
-      <c r="L169" s="14"/>
-      <c r="M169" s="14"/>
-      <c r="N169" s="14"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B170" s="4">
-        <v>6</v>
-      </c>
-      <c r="C170" s="14">
-        <f>RSQ($B$102:$B107, $C$102:$C107)</f>
-        <v>0.96300731041004706</v>
-      </c>
-      <c r="D170" s="14"/>
-      <c r="E170" s="14"/>
-      <c r="F170" s="14"/>
-      <c r="G170" s="14"/>
-      <c r="H170" s="14"/>
-      <c r="I170" s="14"/>
-      <c r="J170" s="14"/>
-      <c r="K170" s="14"/>
-      <c r="L170" s="14"/>
-      <c r="M170" s="14"/>
-      <c r="N170" s="14"/>
+      <c r="A170" t="s">
+        <v>17</v>
+      </c>
+      <c r="C170">
+        <v>11</v>
+      </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>14</v>
+      </c>
       <c r="B171" s="4">
-        <v>7</v>
-      </c>
-      <c r="C171" s="14">
-        <f>RSQ($B$102:$B108, $C$102:$C108)</f>
-        <v>0.95403080349335379</v>
-      </c>
-      <c r="D171" s="14"/>
-      <c r="E171" s="14"/>
-      <c r="F171" s="14"/>
-      <c r="G171" s="14"/>
-      <c r="H171" s="14"/>
-      <c r="I171" s="14"/>
-      <c r="J171" s="14"/>
-      <c r="K171" s="14"/>
-      <c r="L171" s="14"/>
-      <c r="M171" s="14"/>
-      <c r="N171" s="14"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B172" s="4">
-        <v>8</v>
-      </c>
-      <c r="C172" s="14">
-        <f>RSQ($B$102:$B109, $C$102:$C109)</f>
-        <v>0.93978169515797993</v>
-      </c>
-      <c r="D172" s="14"/>
-      <c r="E172" s="14"/>
-      <c r="F172" s="14"/>
-      <c r="G172" s="14"/>
-      <c r="H172" s="14"/>
-      <c r="I172" s="14"/>
-      <c r="J172" s="14"/>
-      <c r="K172" s="14"/>
-      <c r="L172" s="14"/>
-      <c r="M172" s="14"/>
-      <c r="N172" s="14"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B173" s="4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C173" s="14">
-        <f>RSQ($B$102:$B110, $C$102:$C110)</f>
-        <v>0.92541062921847905</v>
-      </c>
+        <f>RSQ($B$109:$B110, $C$109:$C110)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="D173" s="14"/>
+      <c r="E173" s="14"/>
+      <c r="F173" s="14"/>
+      <c r="G173" s="14"/>
+      <c r="H173" s="14"/>
+      <c r="I173" s="14"/>
+      <c r="J173" s="14"/>
+      <c r="K173" s="14"/>
+      <c r="L173" s="14"/>
+      <c r="M173" s="14"/>
+      <c r="N173" s="14"/>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B174" s="5">
-        <v>10</v>
-      </c>
-      <c r="C174" s="14"/>
+      <c r="B174" s="4">
+        <v>3</v>
+      </c>
+      <c r="C174" s="14">
+        <f>RSQ($B$109:$B111, $C$109:$C111)</f>
+        <v>0.99920543508020454</v>
+      </c>
+      <c r="D174" s="14"/>
+      <c r="E174" s="14"/>
+      <c r="F174" s="14"/>
+      <c r="G174" s="14"/>
+      <c r="H174" s="14"/>
+      <c r="I174" s="14"/>
+      <c r="J174" s="14"/>
+      <c r="K174" s="14"/>
+      <c r="L174" s="14"/>
+      <c r="M174" s="14"/>
+      <c r="N174" s="14"/>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B175" s="18">
-        <v>11.5</v>
-      </c>
-      <c r="C175" s="15"/>
+      <c r="B175" s="5">
+        <v>4</v>
+      </c>
+      <c r="C175" s="14">
+        <f>RSQ($B$109:$B112, $C$109:$C112)</f>
+        <v>0.99190519137745259</v>
+      </c>
+      <c r="D175" s="14"/>
+      <c r="E175" s="14"/>
+      <c r="F175" s="14"/>
+      <c r="G175" s="14"/>
+      <c r="H175" s="14"/>
+      <c r="I175" s="14"/>
+      <c r="J175" s="14"/>
+      <c r="K175" s="14"/>
+      <c r="L175" s="14"/>
+      <c r="M175" s="14"/>
+      <c r="N175" s="14"/>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B176" s="4">
+        <v>5</v>
+      </c>
+      <c r="C176" s="14">
+        <f>RSQ($B$109:$B113, $C$109:$C113)</f>
+        <v>0.98056854197001708</v>
+      </c>
+      <c r="D176" s="14"/>
+      <c r="E176" s="14"/>
+      <c r="F176" s="14"/>
+      <c r="G176" s="14"/>
+      <c r="H176" s="14"/>
+      <c r="I176" s="14"/>
+      <c r="J176" s="14"/>
+      <c r="K176" s="14"/>
+      <c r="L176" s="14"/>
+      <c r="M176" s="14"/>
+      <c r="N176" s="14"/>
+    </row>
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B177" s="4">
+        <v>6</v>
+      </c>
+      <c r="C177" s="14">
+        <f>RSQ($B$109:$B114, $C$109:$C114)</f>
+        <v>0.96300731041004706</v>
+      </c>
+      <c r="D177" s="14"/>
+      <c r="E177" s="14"/>
+      <c r="F177" s="14"/>
+      <c r="G177" s="14"/>
+      <c r="H177" s="14"/>
+      <c r="I177" s="14"/>
+      <c r="J177" s="14"/>
+      <c r="K177" s="14"/>
+      <c r="L177" s="14"/>
+      <c r="M177" s="14"/>
+      <c r="N177" s="14"/>
+    </row>
+    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B178" s="4">
+        <v>7</v>
+      </c>
+      <c r="C178" s="14">
+        <f>RSQ($B$109:$B115, $C$109:$C115)</f>
+        <v>0.95403080349335379</v>
+      </c>
+      <c r="D178" s="14"/>
+      <c r="E178" s="14"/>
+      <c r="F178" s="14"/>
+      <c r="G178" s="14"/>
+      <c r="H178" s="14"/>
+      <c r="I178" s="14"/>
+      <c r="J178" s="14"/>
+      <c r="K178" s="14"/>
+      <c r="L178" s="14"/>
+      <c r="M178" s="14"/>
+      <c r="N178" s="14"/>
+    </row>
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B179" s="4">
+        <v>8</v>
+      </c>
+      <c r="C179" s="14">
+        <f>RSQ($B$109:$B116, $C$109:$C116)</f>
+        <v>0.93978169515797993</v>
+      </c>
+      <c r="D179" s="14"/>
+      <c r="E179" s="14"/>
+      <c r="F179" s="14"/>
+      <c r="G179" s="14"/>
+      <c r="H179" s="14"/>
+      <c r="I179" s="14"/>
+      <c r="J179" s="14"/>
+      <c r="K179" s="14"/>
+      <c r="L179" s="14"/>
+      <c r="M179" s="14"/>
+      <c r="N179" s="14"/>
+    </row>
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B180" s="4">
+        <v>9</v>
+      </c>
+      <c r="C180" s="14"/>
+    </row>
+    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B181" s="5">
+        <v>10</v>
+      </c>
+      <c r="C181" s="14"/>
+    </row>
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B182" s="17">
+        <v>11.5</v>
+      </c>
+      <c r="C182" s="15"/>
+    </row>
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B183" s="4">
         <v>13</v>
       </c>
-      <c r="C176" s="14"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="4">
+      <c r="C183" s="14"/>
+    </row>
+    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B184" s="4">
         <v>14.5</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="4">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B185" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="4">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B186" s="4">
         <v>17.5</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="4">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B187" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="4">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B188" s="4">
         <v>20.5</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="4">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B189" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="4">
+    <row r="190" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B190" s="4">
         <v>23.5</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="4">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B191" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="4">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B192" s="4">
         <v>27</v>
-      </c>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="4">
-        <v>41</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" s="4">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" s="4">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>18</v>
-      </c>
       <c r="B195" s="4">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" s="4">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B197" s="4">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" s="4">
-        <v>3</v>
-      </c>
-      <c r="C198">
-        <f>RSQ($B104:$B$111, C104:C$111)</f>
-        <v>0.96098077312371055</v>
+        <v>39</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B199" s="5">
-        <v>4</v>
-      </c>
-      <c r="C199">
-        <f>RSQ($B105:$B$111, C105:C$111)</f>
-        <v>0.97670463102946459</v>
+      <c r="B199" s="4">
+        <v>41</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" s="4">
-        <v>5</v>
-      </c>
-      <c r="C200">
-        <f>RSQ($B106:$B$111, C106:C$111)</f>
-        <v>0.98671006722167587</v>
+        <v>43</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="4">
-        <v>6</v>
-      </c>
-      <c r="C201">
-        <f>RSQ($B107:$B$111, C107:C$111)</f>
-        <v>0.98512380447254111</v>
+        <v>45</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>18</v>
+      </c>
       <c r="B202" s="4">
-        <v>7</v>
-      </c>
-      <c r="C202">
-        <f>RSQ($B108:$B$111, C108:C$111)</f>
-        <v>0.99232975970630322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" s="4">
-        <v>8</v>
-      </c>
-      <c r="C203">
-        <f>RSQ($B109:$B$111, C109:C$111)</f>
-        <v>0.98826903437871538</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B204" s="4">
-        <v>9</v>
-      </c>
-      <c r="C204">
-        <f>RSQ($B110:$B$111, C110:C$111)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B205" s="5">
-        <v>10</v>
+      <c r="B205" s="4">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <f>RSQ($B111:$B$118, C111:C$118)</f>
+        <v>0.96098077312371055</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B206" s="18">
-        <v>11.5</v>
-      </c>
-      <c r="C206" s="19"/>
+      <c r="B206" s="5">
+        <v>4</v>
+      </c>
+      <c r="C206">
+        <f>RSQ($B112:$B$118, C112:C$118)</f>
+        <v>0.97670463102946459</v>
+      </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" s="4">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C207">
+        <f>RSQ($B113:$B$118, C113:C$118)</f>
+        <v>0.98671006722167587</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="4">
+        <v>6</v>
+      </c>
+      <c r="C208">
+        <f>RSQ($B114:$B$118, C114:C$118)</f>
+        <v>0.98512380447254111</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" s="4">
+        <v>7</v>
+      </c>
+      <c r="C209">
+        <f>RSQ($B115:$B$118, C115:C$118)</f>
+        <v>0.99232975970630322</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="4">
+        <v>8</v>
+      </c>
+      <c r="C210">
+        <f>RSQ($B116:$B$118, C116:C$118)</f>
+        <v>0.98826903437871538</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" s="4">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <f>RSQ($B117:$B$118, C117:C$118)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="17">
+        <v>11.5</v>
+      </c>
+      <c r="C213" s="18"/>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="4">
         <v>14.5</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B209" s="4">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B210" s="4">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="4">
         <v>17.5</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B211" s="4">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B212" s="4">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="4">
         <v>20.5</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" s="4">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" s="4">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B221" s="4">
         <v>23.5</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B215" s="4">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B222" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B216" s="4">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B217" s="4">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B224" s="4">
         <v>29</v>
-      </c>
-    </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B218" s="4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B219" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B222" s="4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B223" s="4">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B224" s="4">
-        <v>43</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B225" s="4">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>15</v>
-      </c>
       <c r="B226" s="4">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B227" s="4">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B228" s="4">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B229" s="4">
-        <v>3</v>
-      </c>
-      <c r="C229" s="14">
-        <f>SUM(C166,C198)</f>
-        <v>1.9609807731237103</v>
+        <v>39</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B230" s="5">
-        <v>4</v>
-      </c>
-      <c r="C230" s="14">
-        <f t="shared" ref="C229:C235" si="3">SUM(C167,C199)</f>
-        <v>1.9759100661096691</v>
-      </c>
-      <c r="D230" s="14"/>
-      <c r="E230" s="14"/>
-      <c r="F230" s="14"/>
-      <c r="G230" s="14"/>
-      <c r="H230" s="14"/>
-      <c r="I230" s="14"/>
-      <c r="J230" s="14"/>
-      <c r="K230" s="14"/>
-      <c r="L230" s="14"/>
-      <c r="M230" s="14"/>
-      <c r="N230" s="14"/>
+      <c r="B230" s="4">
+        <v>41</v>
+      </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B231" s="4">
-        <v>5</v>
-      </c>
-      <c r="C231" s="20">
-        <f>SUM(C168,C200)</f>
-        <v>1.9786152585991283</v>
-      </c>
-      <c r="D231" s="14"/>
-      <c r="E231" s="14"/>
-      <c r="F231" s="14"/>
-      <c r="G231" s="14"/>
-      <c r="H231" s="14"/>
-      <c r="I231" s="14"/>
-      <c r="J231" s="14"/>
-      <c r="K231" s="14"/>
-      <c r="L231" s="14"/>
-      <c r="M231" s="14"/>
-      <c r="N231" s="14"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B232" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>15</v>
+      </c>
+      <c r="B233" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B234" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B235" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B236" s="4">
+        <v>3</v>
+      </c>
+      <c r="C236" s="14">
+        <f>SUM(C173,C205)</f>
+        <v>1.9609807731237103</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B237" s="5">
+        <v>4</v>
+      </c>
+      <c r="C237" s="14">
+        <f t="shared" ref="C237:C242" si="3">SUM(C174,C206)</f>
+        <v>1.9759100661096691</v>
+      </c>
+      <c r="D237" s="14"/>
+      <c r="E237" s="14"/>
+      <c r="F237" s="14"/>
+      <c r="G237" s="14"/>
+      <c r="H237" s="14"/>
+      <c r="I237" s="14"/>
+      <c r="J237" s="14"/>
+      <c r="K237" s="14"/>
+      <c r="L237" s="14"/>
+      <c r="M237" s="14"/>
+      <c r="N237" s="14"/>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B238" s="4">
+        <v>5</v>
+      </c>
+      <c r="C238" s="19">
+        <f>SUM(C175,C207)</f>
+        <v>1.9786152585991283</v>
+      </c>
+      <c r="D238" s="14"/>
+      <c r="E238" s="14"/>
+      <c r="F238" s="14"/>
+      <c r="G238" s="14"/>
+      <c r="H238" s="14"/>
+      <c r="I238" s="14"/>
+      <c r="J238" s="14"/>
+      <c r="K238" s="14"/>
+      <c r="L238" s="14"/>
+      <c r="M238" s="14"/>
+      <c r="N238" s="14"/>
+    </row>
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B239" s="4">
         <v>6</v>
       </c>
-      <c r="C232" s="14">
+      <c r="C239" s="14">
         <f t="shared" si="3"/>
         <v>1.9656923464425582</v>
       </c>
-      <c r="D232" s="14"/>
-      <c r="E232" s="14"/>
-      <c r="F232" s="14"/>
-      <c r="G232" s="14"/>
-      <c r="H232" s="14"/>
-      <c r="I232" s="14"/>
-      <c r="J232" s="14"/>
-      <c r="K232" s="14"/>
-      <c r="L232" s="14"/>
-      <c r="M232" s="14"/>
-      <c r="N232" s="14"/>
-    </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B233" s="4">
+      <c r="D239" s="14"/>
+      <c r="E239" s="14"/>
+      <c r="F239" s="14"/>
+      <c r="G239" s="14"/>
+      <c r="H239" s="14"/>
+      <c r="I239" s="14"/>
+      <c r="J239" s="14"/>
+      <c r="K239" s="14"/>
+      <c r="L239" s="14"/>
+      <c r="M239" s="14"/>
+      <c r="N239" s="14"/>
+    </row>
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B240" s="4">
         <v>7</v>
       </c>
-      <c r="C233" s="14">
+      <c r="C240" s="14">
         <f t="shared" si="3"/>
         <v>1.9553370701163502</v>
       </c>
-      <c r="D233" s="14"/>
-      <c r="E233" s="14"/>
-      <c r="F233" s="14"/>
-      <c r="G233" s="14"/>
-      <c r="H233" s="14"/>
-      <c r="I233" s="14"/>
-      <c r="J233" s="14"/>
-      <c r="K233" s="14"/>
-      <c r="L233" s="14"/>
-      <c r="M233" s="14"/>
-      <c r="N233" s="14"/>
-    </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B234" s="4">
+      <c r="D240" s="14"/>
+      <c r="E240" s="14"/>
+      <c r="F240" s="14"/>
+      <c r="G240" s="14"/>
+      <c r="H240" s="14"/>
+      <c r="I240" s="14"/>
+      <c r="J240" s="14"/>
+      <c r="K240" s="14"/>
+      <c r="L240" s="14"/>
+      <c r="M240" s="14"/>
+      <c r="N240" s="14"/>
+    </row>
+    <row r="241" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B241" s="4">
         <v>8</v>
       </c>
-      <c r="C234" s="14">
+      <c r="C241" s="14">
         <f t="shared" si="3"/>
         <v>1.9422998378720693</v>
       </c>
-      <c r="D234" s="14"/>
-      <c r="E234" s="14"/>
-      <c r="F234" s="14"/>
-      <c r="G234" s="14"/>
-      <c r="H234" s="14"/>
-      <c r="I234" s="14"/>
-      <c r="J234" s="14"/>
-      <c r="K234" s="14"/>
-      <c r="L234" s="14"/>
-      <c r="M234" s="14"/>
-      <c r="N234" s="14"/>
-    </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B235" s="4">
+      <c r="D241" s="14"/>
+      <c r="E241" s="14"/>
+      <c r="F241" s="14"/>
+      <c r="G241" s="14"/>
+      <c r="H241" s="14"/>
+      <c r="I241" s="14"/>
+      <c r="J241" s="14"/>
+      <c r="K241" s="14"/>
+      <c r="L241" s="14"/>
+      <c r="M241" s="14"/>
+      <c r="N241" s="14"/>
+    </row>
+    <row r="242" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B242" s="4">
         <v>9</v>
       </c>
-      <c r="C235" s="14">
+      <c r="C242" s="14">
         <f t="shared" si="3"/>
         <v>1.93978169515798</v>
       </c>
-      <c r="D235" s="14"/>
-      <c r="E235" s="14"/>
-      <c r="F235" s="14"/>
-      <c r="G235" s="14"/>
-      <c r="H235" s="14"/>
-      <c r="I235" s="14"/>
-      <c r="J235" s="14"/>
-      <c r="K235" s="14"/>
-      <c r="L235" s="14"/>
-      <c r="M235" s="14"/>
-      <c r="N235" s="14"/>
-    </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B236" s="5">
+      <c r="D242" s="14"/>
+      <c r="E242" s="14"/>
+      <c r="F242" s="14"/>
+      <c r="G242" s="14"/>
+      <c r="H242" s="14"/>
+      <c r="I242" s="14"/>
+      <c r="J242" s="14"/>
+      <c r="K242" s="14"/>
+      <c r="L242" s="14"/>
+      <c r="M242" s="14"/>
+      <c r="N242" s="14"/>
+    </row>
+    <row r="243" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B243" s="5">
         <v>10</v>
       </c>
-      <c r="D236" s="14"/>
-      <c r="E236" s="14"/>
-      <c r="F236" s="14"/>
-      <c r="G236" s="14"/>
-      <c r="H236" s="14"/>
-      <c r="I236" s="14"/>
-      <c r="J236" s="14"/>
-      <c r="K236" s="14"/>
-      <c r="L236" s="14"/>
-      <c r="M236" s="14"/>
-      <c r="N236" s="14"/>
-    </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B237" s="5">
+      <c r="D243" s="14"/>
+      <c r="E243" s="14"/>
+      <c r="F243" s="14"/>
+      <c r="G243" s="14"/>
+      <c r="H243" s="14"/>
+      <c r="I243" s="14"/>
+      <c r="J243" s="14"/>
+      <c r="K243" s="14"/>
+      <c r="L243" s="14"/>
+      <c r="M243" s="14"/>
+      <c r="N243" s="14"/>
+    </row>
+    <row r="244" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B244" s="5">
         <v>11.5</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B238" s="4">
+    <row r="245" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B245" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B239" s="4">
+    <row r="246" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B246" s="4">
         <v>14.5</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B240" s="4">
+    <row r="247" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B247" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B241" s="4">
+    <row r="248" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B248" s="4">
         <v>17.5</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B242" s="4">
+    <row r="249" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B249" s="4">
         <v>19</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B243" s="4">
+    <row r="250" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B250" s="4">
         <v>20.5</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B244" s="4">
+    <row r="251" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B251" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B245" s="4">
+    <row r="252" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B252" s="4">
         <v>23.5</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B246" s="4">
+    <row r="253" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B253" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B247" s="4">
+    <row r="254" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B254" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B248" s="4">
+    <row r="255" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B255" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B249" s="4">
+    <row r="256" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B256" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B250" s="4">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B257" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B251" s="4">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B258" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B252" s="4">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B259" s="4">
         <v>37</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B253" s="4">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B260" s="4">
         <v>39</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B254" s="4">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B261" s="4">
         <v>41</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B255" s="4">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B262" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B256" s="4">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B263" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
         <v>16</v>
       </c>
-      <c r="C257">
-        <f>MAX(C226:C256)</f>
+      <c r="C264">
+        <f>MAX(C233:C263)</f>
         <v>1.9786152585991283</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>19</v>
       </c>
-      <c r="C258">
+      <c r="C265">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="13">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>